<commit_message>
Add example into excel
</commit_message>
<xml_diff>
--- a/handball_analytics.xlsx
+++ b/handball_analytics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aec46fcadf735255/Documents/Projekte/Programmieren/handball_analytics/handball_stats_visualisations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{2ADCC356-E079-4742-A213-8E7E5485BD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E4BA8B8-282C-4CF5-8C8B-A3BC237E9235}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{2ADCC356-E079-4742-A213-8E7E5485BD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25233A44-62FB-454A-A9D9-39C414523572}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="1020" windowWidth="19180" windowHeight="7710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="19180" windowHeight="10890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
   <si>
     <t>Spieler</t>
   </si>
@@ -195,6 +195,30 @@
   </si>
   <si>
     <t>RL_9,14,9;KM,0,0;RA,13,1;KM,8,1;TG,2,1;KM,1,9;TG,2,10;RM_6,13,1;KM,8,1;RA,2,2;RA,2,3;RA,2,6</t>
+  </si>
+  <si>
+    <t>Benutze f2 um in die Zelle zu gehen.</t>
+  </si>
+  <si>
+    <t>Dann wie in der ersten Zeile beschrieben die Daten eingeben.</t>
+  </si>
+  <si>
+    <t>Ein Tor das in der 23 Minute oben rechts in den Winkel geworfen wurde sie dann bspw. so aus:</t>
+  </si>
+  <si>
+    <t>23,15,10;</t>
+  </si>
+  <si>
+    <t>Wenn danach in Minute 24 gleich noch ein Tor geworfen wird, wo der Torwart getunnelt wird macht das:</t>
+  </si>
+  <si>
+    <t>23,15,10;24,8,1;</t>
+  </si>
+  <si>
+    <t>Und sagen wir es läuft grade bei diesem Spieler und er macht noch ein drittes Tor, dieses Mal einen Lupfer noch in der gleichen Minute:</t>
+  </si>
+  <si>
+    <t>23,15,10;24,8,1;24,8,10</t>
   </si>
 </sst>
 </file>
@@ -568,7 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -962,10 +986,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECDCE89-6426-4ACD-B450-AC87F0265085}">
-  <dimension ref="A1:Y13"/>
+  <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -974,6 +998,9 @@
     <col min="5" max="5" width="31.08984375" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="16.1796875" customWidth="1"/>
+    <col min="9" max="9" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="18" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="25" width="2.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
@@ -1361,6 +1388,46 @@
         <v>15</v>
       </c>
     </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>